<commit_message>
Conclusão da CadastroPage referente ao cadastro usando massa do Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/DataAdvantage.xlsx
+++ b/src/test/resources/DataAdvantage.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">postalcode</t>
   </si>
   <si>
-    <t xml:space="preserve">user1Plan</t>
+    <t xml:space="preserve">user4Plan</t>
   </si>
   <si>
     <t xml:space="preserve">user1@btr.com</t>
@@ -76,10 +76,10 @@
     <t xml:space="preserve">Brazil</t>
   </si>
   <si>
-    <t xml:space="preserve">cidade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rua Test, 1</t>
+    <t xml:space="preserve">cidadePlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua Test Plan, 1 </t>
   </si>
   <si>
     <t xml:space="preserve">Sao Paulo</t>
@@ -267,14 +267,16 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>